<commit_message>
update OFT repo with power analysis
</commit_message>
<xml_diff>
--- a/Longitudinal_induction_analysis/OFT/OFT_binned_longitudinal_data.xlsx
+++ b/Longitudinal_induction_analysis/OFT/OFT_binned_longitudinal_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annastuckert/Documents/GitHub/TDPBehaviorAnalysis/Longitudinal_induction_analysis/OFT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8AB547-E8C9-7B4D-AC97-607C9A0D7B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B30B9F-FB1F-5B4F-B622-1294BA5E278E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="500" windowWidth="14740" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12960" yWindow="640" windowWidth="14740" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -101,6 +101,27 @@
   </si>
   <si>
     <t>Timebin 2</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
+    <t>262</t>
+  </si>
+  <si>
+    <t>271</t>
+  </si>
+  <si>
+    <t>281</t>
   </si>
 </sst>
 </file>
@@ -451,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64:B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2553,6 +2574,1728 @@
         <v>14</v>
       </c>
     </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <v>2913.86</v>
+      </c>
+      <c r="D52">
+        <v>9.7212899999999998</v>
+      </c>
+      <c r="E52">
+        <v>231.66</v>
+      </c>
+      <c r="F52">
+        <v>68.28</v>
+      </c>
+      <c r="G52">
+        <v>19</v>
+      </c>
+      <c r="H52">
+        <v>34.18</v>
+      </c>
+      <c r="I52">
+        <v>0.26</v>
+      </c>
+      <c r="J52">
+        <v>20</v>
+      </c>
+      <c r="K52">
+        <v>265.82</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53">
+        <v>2317.94</v>
+      </c>
+      <c r="D53">
+        <v>7.7305999999999999</v>
+      </c>
+      <c r="E53">
+        <v>206.26</v>
+      </c>
+      <c r="F53">
+        <v>93.74</v>
+      </c>
+      <c r="G53">
+        <v>14</v>
+      </c>
+      <c r="H53">
+        <v>30.46</v>
+      </c>
+      <c r="I53">
+        <v>300.39999999999998</v>
+      </c>
+      <c r="J53">
+        <v>15</v>
+      </c>
+      <c r="K53">
+        <v>269.54000000000002</v>
+      </c>
+      <c r="L53">
+        <v>300</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <v>2933.48</v>
+      </c>
+      <c r="D54">
+        <v>9.7854399999999995</v>
+      </c>
+      <c r="E54">
+        <v>250.66</v>
+      </c>
+      <c r="F54">
+        <v>49.28</v>
+      </c>
+      <c r="G54">
+        <v>20</v>
+      </c>
+      <c r="H54">
+        <v>55.98</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>20</v>
+      </c>
+      <c r="K54">
+        <v>244.02</v>
+      </c>
+      <c r="L54">
+        <v>6.12</v>
+      </c>
+      <c r="M54" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55">
+        <v>2160.7399999999998</v>
+      </c>
+      <c r="D55">
+        <v>7.2063100000000002</v>
+      </c>
+      <c r="E55">
+        <v>208.12</v>
+      </c>
+      <c r="F55">
+        <v>91.88</v>
+      </c>
+      <c r="G55">
+        <v>14</v>
+      </c>
+      <c r="H55">
+        <v>41.12</v>
+      </c>
+      <c r="I55">
+        <v>312.32</v>
+      </c>
+      <c r="J55">
+        <v>15</v>
+      </c>
+      <c r="K55">
+        <v>258.88</v>
+      </c>
+      <c r="L55">
+        <v>300</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56">
+        <v>3194.82</v>
+      </c>
+      <c r="D56">
+        <v>10.6572</v>
+      </c>
+      <c r="E56">
+        <v>233.4</v>
+      </c>
+      <c r="F56">
+        <v>66.540000000000006</v>
+      </c>
+      <c r="G56">
+        <v>27</v>
+      </c>
+      <c r="H56">
+        <v>63.48</v>
+      </c>
+      <c r="I56">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="J56">
+        <v>27</v>
+      </c>
+      <c r="K56">
+        <v>236.52</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57">
+        <v>2188.88</v>
+      </c>
+      <c r="D57">
+        <v>7.30016</v>
+      </c>
+      <c r="E57">
+        <v>203.54</v>
+      </c>
+      <c r="F57">
+        <v>96.46</v>
+      </c>
+      <c r="G57">
+        <v>28</v>
+      </c>
+      <c r="H57">
+        <v>86.68</v>
+      </c>
+      <c r="I57">
+        <v>300</v>
+      </c>
+      <c r="J57">
+        <v>28</v>
+      </c>
+      <c r="K57">
+        <v>213.32</v>
+      </c>
+      <c r="L57">
+        <v>301.24</v>
+      </c>
+      <c r="M57" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <v>2386.36</v>
+      </c>
+      <c r="D58">
+        <v>7.9603799999999998</v>
+      </c>
+      <c r="E58">
+        <v>209.28</v>
+      </c>
+      <c r="F58">
+        <v>90.66</v>
+      </c>
+      <c r="G58">
+        <v>21</v>
+      </c>
+      <c r="H58">
+        <v>31.46</v>
+      </c>
+      <c r="I58">
+        <v>68.7</v>
+      </c>
+      <c r="J58">
+        <v>22</v>
+      </c>
+      <c r="K58">
+        <v>268.54000000000002</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59">
+        <v>2779.34</v>
+      </c>
+      <c r="D59">
+        <v>9.2694100000000006</v>
+      </c>
+      <c r="E59">
+        <v>227.46</v>
+      </c>
+      <c r="F59">
+        <v>72.540000000000006</v>
+      </c>
+      <c r="G59">
+        <v>22</v>
+      </c>
+      <c r="H59">
+        <v>47.72</v>
+      </c>
+      <c r="I59">
+        <v>306.12</v>
+      </c>
+      <c r="J59">
+        <v>23</v>
+      </c>
+      <c r="K59">
+        <v>252.28</v>
+      </c>
+      <c r="L59">
+        <v>300</v>
+      </c>
+      <c r="M59" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60">
+        <v>3494.45</v>
+      </c>
+      <c r="D60">
+        <v>11.656700000000001</v>
+      </c>
+      <c r="E60">
+        <v>241.5</v>
+      </c>
+      <c r="F60">
+        <v>58.44</v>
+      </c>
+      <c r="G60">
+        <v>28</v>
+      </c>
+      <c r="H60">
+        <v>50.02</v>
+      </c>
+      <c r="I60">
+        <v>47.72</v>
+      </c>
+      <c r="J60">
+        <v>29</v>
+      </c>
+      <c r="K60">
+        <v>249.98</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61">
+        <v>3082.67</v>
+      </c>
+      <c r="D61">
+        <v>10.281000000000001</v>
+      </c>
+      <c r="E61">
+        <v>244.98</v>
+      </c>
+      <c r="F61">
+        <v>55.02</v>
+      </c>
+      <c r="G61">
+        <v>32</v>
+      </c>
+      <c r="H61">
+        <v>67.319999999999993</v>
+      </c>
+      <c r="I61">
+        <v>301.14</v>
+      </c>
+      <c r="J61">
+        <v>33</v>
+      </c>
+      <c r="K61">
+        <v>232.68</v>
+      </c>
+      <c r="L61">
+        <v>300</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62">
+        <v>2699.73</v>
+      </c>
+      <c r="D62">
+        <v>9.0057100000000005</v>
+      </c>
+      <c r="E62">
+        <v>209.72</v>
+      </c>
+      <c r="F62">
+        <v>90.22</v>
+      </c>
+      <c r="G62">
+        <v>16</v>
+      </c>
+      <c r="H62">
+        <v>23.54</v>
+      </c>
+      <c r="I62">
+        <v>3.06</v>
+      </c>
+      <c r="J62">
+        <v>16</v>
+      </c>
+      <c r="K62">
+        <v>276.45999999999998</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63">
+        <v>3707.65</v>
+      </c>
+      <c r="D63">
+        <v>12.365399999999999</v>
+      </c>
+      <c r="E63">
+        <v>253.18</v>
+      </c>
+      <c r="F63">
+        <v>46.82</v>
+      </c>
+      <c r="G63">
+        <v>35</v>
+      </c>
+      <c r="H63">
+        <v>76.12</v>
+      </c>
+      <c r="I63">
+        <v>300</v>
+      </c>
+      <c r="J63">
+        <v>35</v>
+      </c>
+      <c r="K63">
+        <v>223.88</v>
+      </c>
+      <c r="L63">
+        <v>304.44</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64">
+        <v>3942.98</v>
+      </c>
+      <c r="D64">
+        <v>13.152900000000001</v>
+      </c>
+      <c r="E64">
+        <v>260.5</v>
+      </c>
+      <c r="F64">
+        <v>39.44</v>
+      </c>
+      <c r="G64">
+        <v>42</v>
+      </c>
+      <c r="H64">
+        <v>68.92</v>
+      </c>
+      <c r="I64">
+        <v>16.64</v>
+      </c>
+      <c r="J64">
+        <v>43</v>
+      </c>
+      <c r="K64">
+        <v>231.08</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>26</v>
+      </c>
+      <c r="C65">
+        <v>2932.34</v>
+      </c>
+      <c r="D65">
+        <v>9.7796900000000004</v>
+      </c>
+      <c r="E65">
+        <v>246.06</v>
+      </c>
+      <c r="F65">
+        <v>53.94</v>
+      </c>
+      <c r="G65">
+        <v>45</v>
+      </c>
+      <c r="H65">
+        <v>128.86000000000001</v>
+      </c>
+      <c r="I65">
+        <v>301.5</v>
+      </c>
+      <c r="J65">
+        <v>46</v>
+      </c>
+      <c r="K65">
+        <v>171.14</v>
+      </c>
+      <c r="L65">
+        <v>300</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>2412.31</v>
+      </c>
+      <c r="D66">
+        <v>8.04908</v>
+      </c>
+      <c r="E66">
+        <v>226.84</v>
+      </c>
+      <c r="F66">
+        <v>73.08</v>
+      </c>
+      <c r="G66">
+        <v>20</v>
+      </c>
+      <c r="H66">
+        <v>77.62</v>
+      </c>
+      <c r="I66">
+        <v>1.4</v>
+      </c>
+      <c r="J66">
+        <v>21</v>
+      </c>
+      <c r="K66">
+        <v>222.38</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67">
+        <v>1642.85</v>
+      </c>
+      <c r="D67">
+        <v>5.4790999999999999</v>
+      </c>
+      <c r="E67">
+        <v>196.02</v>
+      </c>
+      <c r="F67">
+        <v>103.98</v>
+      </c>
+      <c r="G67">
+        <v>16</v>
+      </c>
+      <c r="H67">
+        <v>67.12</v>
+      </c>
+      <c r="I67">
+        <v>303.54000000000002</v>
+      </c>
+      <c r="J67">
+        <v>17</v>
+      </c>
+      <c r="K67">
+        <v>232.88</v>
+      </c>
+      <c r="L67">
+        <v>300</v>
+      </c>
+      <c r="M67" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68">
+        <v>1345.08</v>
+      </c>
+      <c r="D68">
+        <v>4.4868800000000002</v>
+      </c>
+      <c r="E68">
+        <v>172.18</v>
+      </c>
+      <c r="F68">
+        <v>127.76</v>
+      </c>
+      <c r="G68">
+        <v>13</v>
+      </c>
+      <c r="H68">
+        <v>141.86000000000001</v>
+      </c>
+      <c r="I68">
+        <v>6.24</v>
+      </c>
+      <c r="J68">
+        <v>13</v>
+      </c>
+      <c r="K68">
+        <v>158.13999999999999</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69">
+        <v>1267.33</v>
+      </c>
+      <c r="D69">
+        <v>4.2266899999999996</v>
+      </c>
+      <c r="E69">
+        <v>179.74</v>
+      </c>
+      <c r="F69">
+        <v>120.26</v>
+      </c>
+      <c r="G69">
+        <v>18</v>
+      </c>
+      <c r="H69">
+        <v>74.08</v>
+      </c>
+      <c r="I69">
+        <v>300</v>
+      </c>
+      <c r="J69">
+        <v>18</v>
+      </c>
+      <c r="K69">
+        <v>225.92</v>
+      </c>
+      <c r="L69">
+        <v>300.44</v>
+      </c>
+      <c r="M69" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70">
+        <v>2414.04</v>
+      </c>
+      <c r="D70">
+        <v>8.0526999999999997</v>
+      </c>
+      <c r="E70">
+        <v>240.54</v>
+      </c>
+      <c r="F70">
+        <v>59.4</v>
+      </c>
+      <c r="G70">
+        <v>34</v>
+      </c>
+      <c r="H70">
+        <v>96.46</v>
+      </c>
+      <c r="I70">
+        <v>0.3</v>
+      </c>
+      <c r="J70">
+        <v>34</v>
+      </c>
+      <c r="K70">
+        <v>203.54</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71">
+        <v>2706.54</v>
+      </c>
+      <c r="D71">
+        <v>9.0266099999999998</v>
+      </c>
+      <c r="E71">
+        <v>254.06</v>
+      </c>
+      <c r="F71">
+        <v>45.94</v>
+      </c>
+      <c r="G71">
+        <v>28</v>
+      </c>
+      <c r="H71">
+        <v>109.04</v>
+      </c>
+      <c r="I71">
+        <v>300</v>
+      </c>
+      <c r="J71">
+        <v>28</v>
+      </c>
+      <c r="K71">
+        <v>190.96</v>
+      </c>
+      <c r="L71">
+        <v>315.02</v>
+      </c>
+      <c r="M71" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72">
+        <v>2245.6</v>
+      </c>
+      <c r="D72">
+        <v>7.4908200000000003</v>
+      </c>
+      <c r="E72">
+        <v>211.22</v>
+      </c>
+      <c r="F72">
+        <v>88.72</v>
+      </c>
+      <c r="G72">
+        <v>18</v>
+      </c>
+      <c r="H72">
+        <v>33.64</v>
+      </c>
+      <c r="I72">
+        <v>5.14</v>
+      </c>
+      <c r="J72">
+        <v>19</v>
+      </c>
+      <c r="K72">
+        <v>266.36</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73">
+        <v>2444.7199999999998</v>
+      </c>
+      <c r="D73">
+        <v>8.1545000000000005</v>
+      </c>
+      <c r="E73">
+        <v>221.8</v>
+      </c>
+      <c r="F73">
+        <v>78.2</v>
+      </c>
+      <c r="G73">
+        <v>31</v>
+      </c>
+      <c r="H73">
+        <v>62.62</v>
+      </c>
+      <c r="I73">
+        <v>308.64</v>
+      </c>
+      <c r="J73">
+        <v>31</v>
+      </c>
+      <c r="K73">
+        <v>237.38</v>
+      </c>
+      <c r="L73">
+        <v>300</v>
+      </c>
+      <c r="M73" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>29</v>
+      </c>
+      <c r="B74" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74">
+        <v>3230.52</v>
+      </c>
+      <c r="D74">
+        <v>10.776300000000001</v>
+      </c>
+      <c r="E74">
+        <v>254.7</v>
+      </c>
+      <c r="F74">
+        <v>45.24</v>
+      </c>
+      <c r="G74">
+        <v>24</v>
+      </c>
+      <c r="H74">
+        <v>46.2</v>
+      </c>
+      <c r="I74">
+        <v>7.26</v>
+      </c>
+      <c r="J74">
+        <v>25</v>
+      </c>
+      <c r="K74">
+        <v>253.8</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" t="s">
+        <v>26</v>
+      </c>
+      <c r="C75">
+        <v>2385.0700000000002</v>
+      </c>
+      <c r="D75">
+        <v>7.9544899999999998</v>
+      </c>
+      <c r="E75">
+        <v>227.52</v>
+      </c>
+      <c r="F75">
+        <v>72.48</v>
+      </c>
+      <c r="G75">
+        <v>23</v>
+      </c>
+      <c r="H75">
+        <v>45.84</v>
+      </c>
+      <c r="I75">
+        <v>321.26</v>
+      </c>
+      <c r="J75">
+        <v>24</v>
+      </c>
+      <c r="K75">
+        <v>254.16</v>
+      </c>
+      <c r="L75">
+        <v>300</v>
+      </c>
+      <c r="M75" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76">
+        <v>2726.74</v>
+      </c>
+      <c r="D76">
+        <v>9.0958199999999998</v>
+      </c>
+      <c r="E76">
+        <v>233.88</v>
+      </c>
+      <c r="F76">
+        <v>66.06</v>
+      </c>
+      <c r="G76">
+        <v>25</v>
+      </c>
+      <c r="H76">
+        <v>63.18</v>
+      </c>
+      <c r="I76">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="J76">
+        <v>26</v>
+      </c>
+      <c r="K76">
+        <v>236.82</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77" t="s">
+        <v>26</v>
+      </c>
+      <c r="C77">
+        <v>1518.15</v>
+      </c>
+      <c r="D77">
+        <v>5.0632099999999998</v>
+      </c>
+      <c r="E77">
+        <v>181</v>
+      </c>
+      <c r="F77">
+        <v>119</v>
+      </c>
+      <c r="G77">
+        <v>17</v>
+      </c>
+      <c r="H77">
+        <v>48.3</v>
+      </c>
+      <c r="I77">
+        <v>323.86</v>
+      </c>
+      <c r="J77">
+        <v>18</v>
+      </c>
+      <c r="K77">
+        <v>251.7</v>
+      </c>
+      <c r="L77">
+        <v>300</v>
+      </c>
+      <c r="M77" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" t="s">
+        <v>25</v>
+      </c>
+      <c r="C78">
+        <v>2631.6</v>
+      </c>
+      <c r="D78">
+        <v>8.7784499999999994</v>
+      </c>
+      <c r="E78">
+        <v>227.36</v>
+      </c>
+      <c r="F78">
+        <v>72.58</v>
+      </c>
+      <c r="G78">
+        <v>37</v>
+      </c>
+      <c r="H78">
+        <v>55.9</v>
+      </c>
+      <c r="I78">
+        <v>3.68</v>
+      </c>
+      <c r="J78">
+        <v>38</v>
+      </c>
+      <c r="K78">
+        <v>244.1</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" t="s">
+        <v>26</v>
+      </c>
+      <c r="C79">
+        <v>1981.8</v>
+      </c>
+      <c r="D79">
+        <v>6.60954</v>
+      </c>
+      <c r="E79">
+        <v>203.16</v>
+      </c>
+      <c r="F79">
+        <v>96.84</v>
+      </c>
+      <c r="G79">
+        <v>32</v>
+      </c>
+      <c r="H79">
+        <v>48.48</v>
+      </c>
+      <c r="I79">
+        <v>306.04000000000002</v>
+      </c>
+      <c r="J79">
+        <v>33</v>
+      </c>
+      <c r="K79">
+        <v>251.52</v>
+      </c>
+      <c r="L79">
+        <v>300</v>
+      </c>
+      <c r="M79" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>32</v>
+      </c>
+      <c r="B80" t="s">
+        <v>25</v>
+      </c>
+      <c r="C80">
+        <v>2327.66</v>
+      </c>
+      <c r="D80">
+        <v>7.76457</v>
+      </c>
+      <c r="E80">
+        <v>227.36</v>
+      </c>
+      <c r="F80">
+        <v>72.58</v>
+      </c>
+      <c r="G80">
+        <v>26</v>
+      </c>
+      <c r="H80">
+        <v>46.3</v>
+      </c>
+      <c r="I80">
+        <v>6.12</v>
+      </c>
+      <c r="J80">
+        <v>26</v>
+      </c>
+      <c r="K80">
+        <v>253.7</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>32</v>
+      </c>
+      <c r="B81" t="s">
+        <v>26</v>
+      </c>
+      <c r="C81">
+        <v>1876.42</v>
+      </c>
+      <c r="D81">
+        <v>6.2580799999999996</v>
+      </c>
+      <c r="E81">
+        <v>215.96</v>
+      </c>
+      <c r="F81">
+        <v>84.04</v>
+      </c>
+      <c r="G81">
+        <v>24</v>
+      </c>
+      <c r="H81">
+        <v>92.48</v>
+      </c>
+      <c r="I81">
+        <v>300</v>
+      </c>
+      <c r="J81">
+        <v>23</v>
+      </c>
+      <c r="K81">
+        <v>207.52</v>
+      </c>
+      <c r="L81">
+        <v>301.27999999999997</v>
+      </c>
+      <c r="M81" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>33</v>
+      </c>
+      <c r="B82" t="s">
+        <v>25</v>
+      </c>
+      <c r="C82">
+        <v>1595.51</v>
+      </c>
+      <c r="D82">
+        <v>5.3222899999999997</v>
+      </c>
+      <c r="E82">
+        <v>133.32</v>
+      </c>
+      <c r="F82">
+        <v>166.62</v>
+      </c>
+      <c r="G82">
+        <v>12</v>
+      </c>
+      <c r="H82">
+        <v>20.84</v>
+      </c>
+      <c r="I82">
+        <v>118.76</v>
+      </c>
+      <c r="J82">
+        <v>13</v>
+      </c>
+      <c r="K82">
+        <v>279.16000000000003</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>33</v>
+      </c>
+      <c r="B83" t="s">
+        <v>26</v>
+      </c>
+      <c r="C83">
+        <v>2569.0700000000002</v>
+      </c>
+      <c r="D83">
+        <v>8.5681200000000004</v>
+      </c>
+      <c r="E83">
+        <v>210.36</v>
+      </c>
+      <c r="F83">
+        <v>89.64</v>
+      </c>
+      <c r="G83">
+        <v>26</v>
+      </c>
+      <c r="H83">
+        <v>60.42</v>
+      </c>
+      <c r="I83">
+        <v>304.64</v>
+      </c>
+      <c r="J83">
+        <v>27</v>
+      </c>
+      <c r="K83">
+        <v>239.58</v>
+      </c>
+      <c r="L83">
+        <v>300</v>
+      </c>
+      <c r="M83" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>29</v>
+      </c>
+      <c r="B84" t="s">
+        <v>25</v>
+      </c>
+      <c r="C84">
+        <v>3506.91</v>
+      </c>
+      <c r="D84">
+        <v>11.6983</v>
+      </c>
+      <c r="E84">
+        <v>253.82</v>
+      </c>
+      <c r="F84">
+        <v>46.1</v>
+      </c>
+      <c r="G84">
+        <v>18</v>
+      </c>
+      <c r="H84">
+        <v>20.66</v>
+      </c>
+      <c r="I84">
+        <v>22.82</v>
+      </c>
+      <c r="J84">
+        <v>19</v>
+      </c>
+      <c r="K84">
+        <v>279.33999999999997</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>29</v>
+      </c>
+      <c r="B85" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85">
+        <v>3499.73</v>
+      </c>
+      <c r="D85">
+        <v>11.672000000000001</v>
+      </c>
+      <c r="E85">
+        <v>261.7</v>
+      </c>
+      <c r="F85">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="G85">
+        <v>25</v>
+      </c>
+      <c r="H85">
+        <v>57.26</v>
+      </c>
+      <c r="I85">
+        <v>330.42</v>
+      </c>
+      <c r="J85">
+        <v>26</v>
+      </c>
+      <c r="K85">
+        <v>242.74</v>
+      </c>
+      <c r="L85">
+        <v>300</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>30</v>
+      </c>
+      <c r="B86" t="s">
+        <v>25</v>
+      </c>
+      <c r="C86">
+        <v>3863.41</v>
+      </c>
+      <c r="D86">
+        <v>12.887499999999999</v>
+      </c>
+      <c r="E86">
+        <v>244.84</v>
+      </c>
+      <c r="F86">
+        <v>55.1</v>
+      </c>
+      <c r="G86">
+        <v>29</v>
+      </c>
+      <c r="H86">
+        <v>42.1</v>
+      </c>
+      <c r="I86">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="J86">
+        <v>30</v>
+      </c>
+      <c r="K86">
+        <v>257.89999999999998</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>30</v>
+      </c>
+      <c r="B87" t="s">
+        <v>26</v>
+      </c>
+      <c r="C87">
+        <v>2440.5300000000002</v>
+      </c>
+      <c r="D87">
+        <v>8.1394400000000005</v>
+      </c>
+      <c r="E87">
+        <v>209.02</v>
+      </c>
+      <c r="F87">
+        <v>90.98</v>
+      </c>
+      <c r="G87">
+        <v>24</v>
+      </c>
+      <c r="H87">
+        <v>42.88</v>
+      </c>
+      <c r="I87">
+        <v>304.88</v>
+      </c>
+      <c r="J87">
+        <v>24</v>
+      </c>
+      <c r="K87">
+        <v>257.12</v>
+      </c>
+      <c r="L87">
+        <v>300</v>
+      </c>
+      <c r="M87" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" t="s">
+        <v>25</v>
+      </c>
+      <c r="C88">
+        <v>2021.8</v>
+      </c>
+      <c r="D88">
+        <v>6.7442700000000002</v>
+      </c>
+      <c r="E88">
+        <v>191.02</v>
+      </c>
+      <c r="F88">
+        <v>108.92</v>
+      </c>
+      <c r="G88">
+        <v>19</v>
+      </c>
+      <c r="H88">
+        <v>46.12</v>
+      </c>
+      <c r="I88">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="J88">
+        <v>20</v>
+      </c>
+      <c r="K88">
+        <v>253.88</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>31</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89">
+        <v>1887.92</v>
+      </c>
+      <c r="D89">
+        <v>6.2964200000000003</v>
+      </c>
+      <c r="E89">
+        <v>212.56</v>
+      </c>
+      <c r="F89">
+        <v>87.44</v>
+      </c>
+      <c r="G89">
+        <v>49</v>
+      </c>
+      <c r="H89">
+        <v>67.959999999999994</v>
+      </c>
+      <c r="I89">
+        <v>312.89999999999998</v>
+      </c>
+      <c r="J89">
+        <v>50</v>
+      </c>
+      <c r="K89">
+        <v>232.04</v>
+      </c>
+      <c r="L89">
+        <v>300</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90" t="s">
+        <v>25</v>
+      </c>
+      <c r="C90">
+        <v>2793.78</v>
+      </c>
+      <c r="D90">
+        <v>9.3194499999999998</v>
+      </c>
+      <c r="E90">
+        <v>249.1</v>
+      </c>
+      <c r="F90">
+        <v>50.84</v>
+      </c>
+      <c r="G90">
+        <v>11</v>
+      </c>
+      <c r="H90">
+        <v>25.5</v>
+      </c>
+      <c r="I90">
+        <v>6.8</v>
+      </c>
+      <c r="J90">
+        <v>12</v>
+      </c>
+      <c r="K90">
+        <v>274.5</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>32</v>
+      </c>
+      <c r="B91" t="s">
+        <v>26</v>
+      </c>
+      <c r="C91">
+        <v>2708.98</v>
+      </c>
+      <c r="D91">
+        <v>9.0347399999999993</v>
+      </c>
+      <c r="E91">
+        <v>256.54000000000002</v>
+      </c>
+      <c r="F91">
+        <v>43.46</v>
+      </c>
+      <c r="G91">
+        <v>37</v>
+      </c>
+      <c r="H91">
+        <v>91.44</v>
+      </c>
+      <c r="I91">
+        <v>317.7</v>
+      </c>
+      <c r="J91">
+        <v>38</v>
+      </c>
+      <c r="K91">
+        <v>208.56</v>
+      </c>
+      <c r="L91">
+        <v>300</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" t="s">
+        <v>25</v>
+      </c>
+      <c r="C92">
+        <v>1330.4</v>
+      </c>
+      <c r="D92">
+        <v>4.4379200000000001</v>
+      </c>
+      <c r="E92">
+        <v>130.76</v>
+      </c>
+      <c r="F92">
+        <v>169.18</v>
+      </c>
+      <c r="G92">
+        <v>9</v>
+      </c>
+      <c r="H92">
+        <v>14.26</v>
+      </c>
+      <c r="I92">
+        <v>55.12</v>
+      </c>
+      <c r="J92">
+        <v>10</v>
+      </c>
+      <c r="K92">
+        <v>285.74</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>33</v>
+      </c>
+      <c r="B93" t="s">
+        <v>26</v>
+      </c>
+      <c r="C93">
+        <v>3192.26</v>
+      </c>
+      <c r="D93">
+        <v>10.6465</v>
+      </c>
+      <c r="E93">
+        <v>239.24</v>
+      </c>
+      <c r="F93">
+        <v>60.76</v>
+      </c>
+      <c r="G93">
+        <v>41</v>
+      </c>
+      <c r="H93">
+        <v>51.02</v>
+      </c>
+      <c r="I93">
+        <v>306.33999999999997</v>
+      </c>
+      <c r="J93">
+        <v>42</v>
+      </c>
+      <c r="K93">
+        <v>248.98</v>
+      </c>
+      <c r="L93">
+        <v>300</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>